<commit_message>
item-based user data reduced
</commit_message>
<xml_diff>
--- a/data/Item_based_patents.xlsx
+++ b/data/Item_based_patents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ruchika Ms\CMPE256\Group project\Repo\Recommender-System\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8647368-4F79-4409-BF65-B6930BBA7D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D39A7C6-82CA-40C7-8067-C0BD448D7062}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,25 +60,25 @@
     <t>U08</t>
   </si>
   <si>
-    <t>10349422, 10349418, 10349295</t>
-  </si>
-  <si>
-    <t>10346095, 10346094, 10346083</t>
-  </si>
-  <si>
-    <t>9967960, 9967646, 9967292</t>
-  </si>
-  <si>
-    <t>10331583, 10327202, 10326741, 10326673</t>
-  </si>
-  <si>
     <t>9794808, 9794797</t>
   </si>
   <si>
-    <t>10312751, 10312750, 10312749</t>
-  </si>
-  <si>
-    <t>9967277, 9965766, 9961198</t>
+    <t>10349422, 10349418</t>
+  </si>
+  <si>
+    <t>10346095, 10346094</t>
+  </si>
+  <si>
+    <t>10331583, 10327202</t>
+  </si>
+  <si>
+    <t>10312751, 10312750</t>
+  </si>
+  <si>
+    <t>9967277, 9965766</t>
+  </si>
+  <si>
+    <t>9967960, 9967646</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.1484375" defaultRowHeight="15.6"/>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -517,7 +517,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -526,7 +526,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
     </row>

</xml_diff>